<commit_message>
Notes : Delete MOY column from all files
</commit_message>
<xml_diff>
--- a/resources/G3EI1/notes.xlsx
+++ b/resources/G3EI1/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\G3EI1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE7A97C-7798-4517-8A7C-716E7A6525AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAE76D-1A7F-4412-85BF-1EC2736F089D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>CNE</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>Roelofs</t>
-  </si>
-  <si>
-    <t>MOY</t>
   </si>
   <si>
     <t>Note_G3EI111</t>
@@ -699,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -711,10 +708,9 @@
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="15" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,46 +721,43 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>99</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>101</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>104</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>105</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>106</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>107</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>108</v>
       </c>
-      <c r="O1" t="s">
-        <v>109</v>
-      </c>
-      <c r="P1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -810,12 +803,8 @@
       <c r="O2">
         <v>12</v>
       </c>
-      <c r="P2">
-        <f>AVERAGE(D2:O2)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -861,12 +850,8 @@
       <c r="O3">
         <v>12</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P48" si="0">AVERAGE(D3:O3)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -912,12 +897,8 @@
       <c r="O4">
         <v>12</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -963,12 +944,8 @@
       <c r="O5">
         <v>12</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1014,12 +991,8 @@
       <c r="O6">
         <v>12</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1065,12 +1038,8 @@
       <c r="O7">
         <v>12</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1116,12 +1085,8 @@
       <c r="O8">
         <v>12</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1167,12 +1132,8 @@
       <c r="O9">
         <v>12</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1218,12 +1179,8 @@
       <c r="O10">
         <v>12</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1269,12 +1226,8 @@
       <c r="O11">
         <v>12</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1320,12 +1273,8 @@
       <c r="O12">
         <v>12</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1371,12 +1320,8 @@
       <c r="O13">
         <v>12</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1422,12 +1367,8 @@
       <c r="O14">
         <v>12</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1473,12 +1414,8 @@
       <c r="O15">
         <v>12</v>
       </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1524,12 +1461,8 @@
       <c r="O16">
         <v>12</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1575,12 +1508,8 @@
       <c r="O17">
         <v>12</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1626,12 +1555,8 @@
       <c r="O18">
         <v>12</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1677,12 +1602,8 @@
       <c r="O19">
         <v>12</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1728,12 +1649,8 @@
       <c r="O20">
         <v>12</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1779,12 +1696,8 @@
       <c r="O21">
         <v>12</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1830,12 +1743,8 @@
       <c r="O22">
         <v>12</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1881,12 +1790,8 @@
       <c r="O23">
         <v>12</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1932,12 +1837,8 @@
       <c r="O24">
         <v>12</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1983,12 +1884,8 @@
       <c r="O25">
         <v>12</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2034,12 +1931,8 @@
       <c r="O26">
         <v>12</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2085,12 +1978,8 @@
       <c r="O27">
         <v>12</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2136,12 +2025,8 @@
       <c r="O28">
         <v>12</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2187,12 +2072,8 @@
       <c r="O29">
         <v>12</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2238,12 +2119,8 @@
       <c r="O30">
         <v>12</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2289,12 +2166,8 @@
       <c r="O31">
         <v>12</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2340,12 +2213,8 @@
       <c r="O32">
         <v>12</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2391,12 +2260,8 @@
       <c r="O33">
         <v>12</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2442,12 +2307,8 @@
       <c r="O34">
         <v>12</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2493,12 +2354,8 @@
       <c r="O35">
         <v>12</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2544,12 +2401,8 @@
       <c r="O36">
         <v>12</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2595,12 +2448,8 @@
       <c r="O37">
         <v>12</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2646,12 +2495,8 @@
       <c r="O38">
         <v>12</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2697,12 +2542,8 @@
       <c r="O39">
         <v>12</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2748,12 +2589,8 @@
       <c r="O40">
         <v>12</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2799,12 +2636,8 @@
       <c r="O41">
         <v>12</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2850,12 +2683,8 @@
       <c r="O42">
         <v>12</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2901,12 +2730,8 @@
       <c r="O43">
         <v>12</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2952,12 +2777,8 @@
       <c r="O44">
         <v>12</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3003,12 +2824,8 @@
       <c r="O45">
         <v>12</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3054,12 +2871,8 @@
       <c r="O46">
         <v>12</v>
       </c>
-      <c r="P46">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3105,12 +2918,8 @@
       <c r="O47">
         <v>12</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3154,10 +2963,6 @@
         <v>12</v>
       </c>
       <c r="O48">
-        <v>12</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>

</xml_diff>